<commit_message>
Tez outline devam & sync.
</commit_message>
<xml_diff>
--- a/Project/3501/Furkan/IMMD Production/Gate Driver Test Sonuçları.xlsx
+++ b/Project/3501/Furkan/IMMD Production/Gate Driver Test Sonuçları.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="228">
   <si>
     <t>Test Edilecek Birim</t>
   </si>
@@ -702,6 +702,12 @@
   </si>
   <si>
     <t>Opamp tasarımı düzeltilecek</t>
+  </si>
+  <si>
+    <t>LED'lere yeni renkler eklenecek (şematik)</t>
+  </si>
+  <si>
+    <t>Diyotlara yeni paket (SOT23-3 olacak)</t>
   </si>
 </sst>
 </file>
@@ -814,10 +820,25 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Kötü" xfId="1" builtinId="27"/>
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -834,21 +855,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -883,7 +889,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="tr-TR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2217,7 +2223,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3518,7 +3523,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tablo1" displayName="Tablo1" ref="A1:G109" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tablo1" displayName="Tablo1" ref="A1:G109" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A1:G109"/>
   <tableColumns count="7">
     <tableColumn id="1" name="No"/>
@@ -3534,17 +3539,17 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table1" displayName="Table1" ref="A1:F42" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table1" displayName="Table1" ref="A1:F42" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A1:F42"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Akım"/>
-    <tableColumn id="6" name="Input Voltage(mV)" dataDxfId="5">
+    <tableColumn id="6" name="Input Voltage(mV)" dataDxfId="4">
       <calculatedColumnFormula>A2*4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Voutp" dataDxfId="4"/>
-    <tableColumn id="3" name="Voutn" dataDxfId="3"/>
-    <tableColumn id="4" name="Diff. Amp. Out" dataDxfId="2"/>
-    <tableColumn id="5" name="Expected Diff. Amp. Out" dataDxfId="1">
+    <tableColumn id="2" name="Voutp" dataDxfId="3"/>
+    <tableColumn id="3" name="Voutn" dataDxfId="2"/>
+    <tableColumn id="4" name="Diff. Amp. Out" dataDxfId="1"/>
+    <tableColumn id="5" name="Expected Diff. Amp. Out" dataDxfId="0">
       <calculatedColumnFormula>2*(Table1[[#This Row],[Voutn]]-Table1[[#This Row],[Voutp]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3553,7 +3558,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3820,8 +3825,8 @@
   </sheetPr>
   <dimension ref="A1:H109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+    <sheetView tabSelected="1" topLeftCell="C33" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4522,6 +4527,9 @@
       <c r="G32" t="s">
         <v>192</v>
       </c>
+      <c r="H32" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
@@ -4754,6 +4762,9 @@
       <c r="F42" s="7"/>
       <c r="G42" s="7" t="s">
         <v>199</v>
+      </c>
+      <c r="H42" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>